<commit_message>
UPDATE Prjektplan -  Zielhierarchie
</commit_message>
<xml_diff>
--- a/notizen/Projektplan.xlsx
+++ b/notizen/Projektplan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\Desktop\Entwicklungsprojekt interaktiver Systeme\work in progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\Desktop\Entwicklungsprojekt interaktiver Systeme\Projekt\EISWS1718FuchshoferFonsecaLuis\notizen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>Datum/KW</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Projektplan erstellen</t>
   </si>
   <si>
-    <t>Rapid Prototype erstellen anhand PoC</t>
-  </si>
-  <si>
     <t>MS2</t>
   </si>
   <si>
@@ -258,6 +255,12 @@
   </si>
   <si>
     <t>ABGABE: 28.01.2018</t>
+  </si>
+  <si>
+    <t>Zielhierarchie aufstellen</t>
+  </si>
+  <si>
+    <t>Rapid Prototype erstellen</t>
   </si>
 </sst>
 </file>
@@ -846,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE2A911-F2D5-4AA1-81C0-29AA74D5DCE6}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.7109375" defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -883,7 +886,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -899,10 +902,10 @@
     </row>
     <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -1053,7 +1056,7 @@
     </row>
     <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>20</v>
@@ -1110,26 +1113,26 @@
       <c r="B17" s="6"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="16"/>
+      <c r="H17" s="16">
+        <v>4</v>
+      </c>
       <c r="I17" s="17"/>
     </row>
     <row r="18" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10" t="s">
-        <v>47</v>
-      </c>
+      <c r="D18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="16">
-        <v>8</v>
-      </c>
+      <c r="H18" s="16"/>
       <c r="I18" s="17"/>
     </row>
     <row r="19" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1137,12 +1140,12 @@
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I19" s="17"/>
     </row>
@@ -1151,65 +1154,65 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="16"/>
+      <c r="H21" s="16">
+        <v>1</v>
+      </c>
       <c r="I21" s="17"/>
     </row>
     <row r="22" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="D22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="16">
-        <v>6</v>
-      </c>
+      <c r="H22" s="16"/>
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="16"/>
+      <c r="H23" s="16">
+        <v>6</v>
+      </c>
       <c r="I23" s="17"/>
     </row>
     <row r="24" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="D24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="16">
-        <v>4</v>
-      </c>
+      <c r="H24" s="16"/>
       <c r="I24" s="17"/>
     </row>
     <row r="25" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1217,7 +1220,7 @@
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -1228,35 +1231,35 @@
     </row>
     <row r="26" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
-      <c r="C26" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="16"/>
+      <c r="H26" s="16">
+        <v>4</v>
+      </c>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="C27" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="16">
-        <v>6</v>
-      </c>
+      <c r="H27" s="16"/>
       <c r="I27" s="17"/>
     </row>
     <row r="28" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -1268,93 +1271,95 @@
     </row>
     <row r="29" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
-      <c r="C29" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="16">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I29" s="17"/>
     </row>
     <row r="30" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="16">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="16">
+        <v>3</v>
+      </c>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="16">
         <v>6</v>
       </c>
-      <c r="I31" s="17"/>
-    </row>
-    <row r="32" spans="2:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="7"/>
-      <c r="C32" s="11" t="s">
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="7"/>
+      <c r="C33" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="18">
+        <v>12</v>
+      </c>
+      <c r="I33" s="19"/>
+    </row>
+    <row r="34" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="18">
-        <v>12</v>
-      </c>
-      <c r="I32" s="19"/>
-    </row>
-    <row r="33" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="21"/>
-    </row>
-    <row r="34" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="17"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="21"/>
     </row>
     <row r="35" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="C35" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -1364,15 +1369,13 @@
     <row r="36" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="D36" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="16">
-        <v>12</v>
-      </c>
+      <c r="H36" s="16"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1380,59 +1383,61 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="16">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I37" s="17"/>
     </row>
     <row r="38" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
-      <c r="C38" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="C38" s="10"/>
       <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
+      <c r="E38" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
-      <c r="H38" s="16"/>
+      <c r="H38" s="16">
+        <v>10</v>
+      </c>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="C39" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="16">
-        <v>20</v>
-      </c>
+      <c r="H39" s="16"/>
       <c r="I39" s="17"/>
     </row>
     <row r="40" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="10"/>
+      <c r="D40" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
-      <c r="H40" s="16"/>
+      <c r="H40" s="16">
+        <v>20</v>
+      </c>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="C41" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -1442,15 +1447,13 @@
     <row r="42" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="D42" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="16">
-        <v>10</v>
-      </c>
+      <c r="H42" s="16"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1458,7 +1461,7 @@
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -1469,36 +1472,38 @@
     </row>
     <row r="44" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
-      <c r="C44" s="10" t="s">
-        <v>73</v>
-      </c>
+      <c r="C44" s="10"/>
       <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
+      <c r="E44" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
       <c r="H44" s="16">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="C45" s="10" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="16"/>
+      <c r="H45" s="16">
+        <v>4</v>
+      </c>
       <c r="I45" s="17"/>
     </row>
     <row r="46" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="C46" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
@@ -1508,15 +1513,13 @@
     <row r="47" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="D47" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="10"/>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
-      <c r="H47" s="16">
-        <v>6</v>
-      </c>
+      <c r="H47" s="16"/>
       <c r="I47" s="17"/>
     </row>
     <row r="48" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1524,26 +1527,26 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="16">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I48" s="17"/>
     </row>
     <row r="49" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="C49" s="10"/>
-      <c r="D49" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="16">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I49" s="17"/>
     </row>
@@ -1551,7 +1554,7 @@
       <c r="B50" s="6"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
@@ -1565,34 +1568,36 @@
       <c r="B51" s="6"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
       <c r="H51" s="16">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I51" s="17"/>
     </row>
     <row r="52" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
-      <c r="C52" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
-      <c r="H52" s="16"/>
+      <c r="H52" s="16">
+        <v>6</v>
+      </c>
       <c r="I52" s="17"/>
     </row>
     <row r="53" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10" t="s">
-        <v>55</v>
-      </c>
+      <c r="C53" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
@@ -1602,10 +1607,10 @@
     <row r="54" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10" t="s">
-        <v>56</v>
-      </c>
+      <c r="D54" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="16"/>
@@ -1615,14 +1620,12 @@
       <c r="B55" s="6"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10" t="s">
-        <v>66</v>
-      </c>
+      <c r="E55" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F55" s="10"/>
       <c r="G55" s="10"/>
-      <c r="H55" s="16">
-        <v>7</v>
-      </c>
+      <c r="H55" s="16"/>
       <c r="I55" s="17"/>
     </row>
     <row r="56" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1631,11 +1634,11 @@
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
       <c r="F56" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G56" s="10"/>
       <c r="H56" s="16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I56" s="17"/>
     </row>
@@ -1645,7 +1648,7 @@
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
       <c r="F57" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G57" s="10"/>
       <c r="H57" s="16">
@@ -1659,87 +1662,87 @@
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
       <c r="F58" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G58" s="10"/>
       <c r="H58" s="16">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I58" s="17"/>
     </row>
     <row r="59" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
-      <c r="C59" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
+      <c r="F59" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="G59" s="10"/>
-      <c r="H59" s="16"/>
+      <c r="H59" s="16">
+        <v>15</v>
+      </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="7"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11" t="s">
+    <row r="60" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="6"/>
+      <c r="C60" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="17"/>
+    </row>
+    <row r="61" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="7"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="18">
+        <v>10</v>
+      </c>
+      <c r="I61" s="19"/>
+    </row>
+    <row r="62" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="18">
-        <v>10</v>
-      </c>
-      <c r="I60" s="19"/>
-    </row>
-    <row r="61" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="21"/>
-    </row>
-    <row r="62" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="6"/>
-      <c r="C62" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="16">
-        <v>400</v>
-      </c>
-      <c r="I62" s="17"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="21"/>
     </row>
     <row r="63" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="C63" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
       <c r="H63" s="16">
-        <v>2</v>
+        <v>400</v>
       </c>
       <c r="I63" s="17"/>
     </row>
     <row r="64" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="C64" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
@@ -1750,68 +1753,71 @@
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="7"/>
-      <c r="C65" s="11" t="s">
+    <row r="65" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="6"/>
+      <c r="C65" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="16">
+        <v>2</v>
+      </c>
+      <c r="I65" s="17"/>
+    </row>
+    <row r="66" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="7"/>
+      <c r="C66" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="18">
+        <v>4</v>
+      </c>
+      <c r="I66" s="19"/>
+    </row>
+    <row r="67" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="18">
-        <v>4</v>
-      </c>
-      <c r="I65" s="19"/>
-    </row>
-    <row r="66" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="8" t="s">
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="20">
+        <v>3</v>
+      </c>
+      <c r="I67" s="21"/>
+    </row>
+    <row r="68" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="15">
+        <v>42771</v>
+      </c>
+      <c r="B68" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="20">
-        <v>3</v>
-      </c>
-      <c r="I66" s="21"/>
-    </row>
-    <row r="67" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="15">
-        <v>42771</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="18">
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="18">
         <v>2</v>
       </c>
-      <c r="I67" s="19"/>
-    </row>
-    <row r="68" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="10"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-    </row>
-    <row r="69" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="10"/>
+      <c r="I68" s="19"/>
+    </row>
+    <row r="69" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
@@ -1819,13 +1825,10 @@
       <c r="E70" s="10"/>
       <c r="F70" s="10"/>
       <c r="G70" s="10"/>
-      <c r="H70" s="23">
-        <f>SUM(H1:H67)</f>
-        <v>660</v>
-      </c>
-      <c r="I70" s="21"/>
-    </row>
-    <row r="71" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+    </row>
+    <row r="71" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
@@ -1833,14 +1836,13 @@
       <c r="E71" s="10"/>
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
-      <c r="H71" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="I71" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="23">
+        <f>SUM(H1:H68)</f>
+        <v>664</v>
+      </c>
+      <c r="I71" s="21"/>
+    </row>
+    <row r="72" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="10"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
@@ -1848,6 +1850,12 @@
       <c r="E72" s="10"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
+      <c r="H72" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I72" s="19" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="73" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
@@ -1858,6 +1866,15 @@
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
     </row>
+    <row r="74" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>